<commit_message>
feat: Menambahkan fitur scraping dan pembaruan data koordinat sekolah      Kalipuro    2    3 - Menambahkan script dan notebook baru untuk scraping koordinat sekola      (`scrap_koordinat_sekolah.ipynb`, `scrap_location_sekolah.ipynb`,      `scrape_koordinat_sekolah_new.py`) serta data usaha di kecamatan      Kalipuro (`bps_scrap_koordinat_kec_kalipuro.ipynb`).    4 - Mengimplementasikan hasil scraping baru ke dalam berbagai file Excel      (`database_sekolah_banyuwangi.xlsx`,      `hasil_koordinat_kalipuro_auto_deteksi.xlsx`, dll).    5 - Memperbarui beberapa file data yang sudah ada      (`bps_scrap_koordinat.ipynb`, `data_bisnis_bwi.xlsx`,      `database_cafe_bwi_COMPLETE.xlsx`, `srape_caffe_banyuwangi.ipynb`).    6 - Melakukan update pada `.gitignore` dan `requirements.txt` untuk      mengakomodasi dependensi dan file baru.
</commit_message>
<xml_diff>
--- a/BPS/database_cafe_bwi_COMPLETE.xlsx
+++ b/BPS/database_cafe_bwi_COMPLETE.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,51 +458,51 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tomoro Coffee and Pastry Sudirman, Banyuwangi</t>
+          <t>Bimbel Brain Academy Ruangguru Banyuwangi Genteng</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Jl. Panglima Besar Sudirman No.69, Panderejo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68432</t>
+          <t>Jl. Gajah Mada No.281, Dusun Krajan, Genteng Kulon, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Tomoro+Coffee+and+Pastry+Sudirman,+Banyuwangi/data=!4m7!3m6!1s0x2dd1451614e68805:0x8115ecdfcc9342a5!8m2!3d-8.212793!4d114.3714379!16s%2Fg%2F11w22bn5c3!19sChIJBYjmFBZF0S0RpUKTzN_sFYE?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/Bimbel+Brain+Academy+Ruangguru+Banyuwangi+Genteng/data=!4m7!3m6!1s0x2dd1550077fa80b5:0x76d13d8f2828eda7!8m2!3d-8.3649953!4d114.1446321!16s%2Fg%2F11vzyzl1ly!19sChIJtYD6dwBV0S0Rp-0oKI890XY?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Zazito Co-Working Cafe</t>
+          <t>SERASI - Sekolah Ramah Inklusi</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>5,0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jl. Karang Asem Jl. Tunggul Ametung Gg. I No.02, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>depan TK Aisiyah 1, Jl. Adi Sucipto Belakang masjid Ahmad Dahlan No.18, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Zazito+Co-Working+Cafe/data=!4m7!3m6!1s0x2dd15bf5f12deb21:0x3c4a105222a88400!8m2!3d-8.2242571!4d114.3581515!16s%2Fg%2F11px9_gylw!19sChIJIest8fVb0S0RAISoIlIQSjw?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SERASI+-+Sekolah+Ramah+Inklusi/data=!4m7!3m6!1s0x2dd15ba296dde217:0x7705fe220a4b6031!8m2!3d-8.2282336!4d114.3645804!16s%2Fg%2F11vpr2ps60!19sChIJF-LdlqJb0S0RMWBLCiL-BXc?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D&amp;A Cafe</t>
+          <t>Universitas Dr. Soekardjo (UNIDSOE)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,1002 +512,2564 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jl. Kepiting No.60, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Letkol Istiqlah No.109, Lingkungan Mojoroto R, Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68422</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/D%26A+Cafe/data=!4m7!3m6!1s0x2dd15b013d6762cd:0xdabd44035b4730f1!8m2!3d-8.229541!4d114.3679523!16s%2Fg%2F11pr2_hsgc!19sChIJzWJnPQFb0S0R8TBHWwNEvdo?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/Universitas+Dr.+Soekardjo+%28UNIDSOE%29/data=!4m7!3m6!1s0x2dd145395a7b1b69:0x5be904a98d74cbb6!8m2!3d-8.2064171!4d114.3601024!16s%2Fg%2F11cn5rnvnd!19sChIJaRt7WjlF0S0Rtst0jakE6Vs?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sowan coffee</t>
+          <t>SMK PGRI 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,8</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Kp. Melayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68419</t>
+          <t>Jl. Kepiting No.1, Sobo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Sowan+coffee/data=!4m7!3m6!1s0x2dd1458aac434909:0x681024eacd0f41bf!8m2!3d-8.2066671!4d114.378224!16s%2Fg%2F11mnkntnhh!19sChIJCUlDrIpF0S0Rv0EPzeokEGg?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+PGRI+1+Banyuwangi/data=!4m7!3m6!1s0x2dd15ac68fe7ff9d:0x4f2944699ec84dc8!8m2!3d-8.2346528!4d114.3628124!16s%2Fg%2F1hm5vsvlm!19sChIJnf_nj8Za0S0RyE3InmlEKU8?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>House Of Coffee Banyuwangi</t>
+          <t>SMK Gajah Mada Banyuwangi</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,6</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jl. Brigjen Katamso No.24, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Jaksa Agung Suprapto No.68, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/House+Of+Coffee+Banyuwangi/data=!4m7!3m6!1s0x2dd15b4cf00e3e45:0xa4594b5ed256d2c5!8m2!3d-8.2271215!4d114.3686691!16s%2Fg%2F11j9chx_63!19sChIJRT4O8Exb0S0RxdJW0l5LWaQ?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+Gajah+Mada+Banyuwangi/data=!4m7!3m6!1s0x2dd14536bf8c72b7:0x922cf4ca2f6c195b!8m2!3d-8.2149033!4d114.3624118!16s%2Fg%2F1hm2qpql2!19sChIJt3KMvzZF0S0RWxlsL8r0LJI?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ndalem Coffee And Roastery Kalasan</t>
+          <t>SMK Negeri 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jl. Kalasan No.5, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68419</t>
+          <t>Jl. Wijaya Kusuma No.46, Mojopanggung, GIri, Lingkungan Cuking Rw., Mojopanggung, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68425</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ndalem+Coffee+And+Roastery+Kalasan/data=!4m7!3m6!1s0x2dd15b85bb8b3293:0x65853a3319887612!8m2!3d-8.2171925!4d114.3663761!16s%2Fg%2F11h92dhj2y!19sChIJkzKLu4Vb0S0REnaIGTM6hWU?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+Negeri+1+Banyuwangi/data=!4m7!3m6!1s0x2dd14ff70f397b65:0xd4855a1d5d5b2480!8m2!3d-8.211937!4d114.350435!16s%2Fg%2F11bv355y29!19sChIJZXs5D_dP0S0RgCRbXR1ahdQ?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DKINGS BARBERSHOP CAFE &amp; EATERY</t>
+          <t>Akademi Kelautan Banyuwangi</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Jl. Adi Sucipto No.96, Sobo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
+          <t>JL. Transmigrasi No.5, Lkr. Kp. Baru, Bulusan, Kec. Kalipuro, Kabupaten Banyuwangi, Jawa Timur 68455</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/DKINGS+BARBERSHOP+CAFE+%26+EATERY/data=!4m7!3m6!1s0x2dd15b569cbc1cc1:0x773f1e25143e952c!8m2!3d-8.2333632!4d114.3603334!16s%2Fg%2F11lv7lq4xy!19sChIJwRy8nFZb0S0RLJU-FCUeP3c?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/Akademi+Kelautan+Banyuwangi/data=!4m7!3m6!1s0x2dd14684b01b68e3:0xb0475c52a9bb9a61!8m2!3d-8.1333926!4d114.3925675!16s%2Fg%2F1pzwxv6md!19sChIJ42gbsIRG0S0RYZq7qVJcR7A?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Steven Coffee</t>
+          <t>SMK Pradana Giri Banyuwangi</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Jl. Kolonel Sugiono No.11, Kertosari, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Jaksa Agung Suprapto No.140, Lingkungan Cuking Rw., Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Steven+Coffee/data=!4m7!3m6!1s0x2dd15b098b44c91b:0x9648977e6b56e33a!8m2!3d-8.2268183!4d114.3704586!16s%2Fg%2F11nxvw3nbs!19sChIJG8lEiwlb0S0ROuNWa36XSJY?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+Pradana+Giri+Banyuwangi/data=!4m7!3m6!1s0x2dd14549c231a7cf:0x2f9de34c17999a5d!8m2!3d-8.2156069!4d114.3570054!16s%2Fg%2F11dd_qyxx1!19sChIJz6cxwklF0S0RXZqZF0zjnS8?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Distrik19 Banyuwangi</t>
+          <t>Sekolah Tunas Zaitun Bwi</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4,9</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Pasar Pujasera, Jl. Ikan Mas, Karangrejo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68414</t>
+          <t>Q9J5+64P, Jl. Mendut, Lingkungan Cuking Rw., Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Distrik19+Banyuwangi/data=!4m7!3m6!1s0x2dd1457b4b868f6b:0x10a366e34d898134!8m2!3d-8.2172098!4d114.3762639!16s%2Fg%2F11q1lv64wm!19sChIJa4-GS3tF0S0RNIGJTeNmoxA?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/Sekolah+Tunas+Zaitun+Bwi/data=!4m7!3m6!1s0x2dd14535077a8609:0xe80845b16de0c042!8m2!3d-8.2194043!4d114.3578127!16s%2Fg%2F11bc8zvr3d!19sChIJCYZ6BzVF0S0RQsDgbbFFCOg?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Kopi Om Kim</t>
+          <t>SMK PGRI 2 Giri Banyuwangi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,4</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jl. Simpang Gajah Mada No.3, Lingkungan Cuking Rw., Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68425</t>
+          <t>Jl. Mawar No. 16, Kel. Penataban, Kec. Giri, Lingkungan Mojoroto R, Mojopanggung, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68422</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Kopi+Om+Kim/data=!4m7!3m6!1s0x2dd14519c3fc5363:0x210af3b2c9a5fe36!8m2!3d-8.211355!4d114.3543659!16s%2Fg%2F11hd_m5jzm!19sChIJY1P8wxlF0S0RNv6lybLzCiE?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+PGRI+2+Giri+Banyuwangi/data=!4m7!3m6!1s0x2dd145416b71143d:0x6cad4b26d34c9214!8m2!3d-8.2052687!4d114.3544076!16s%2Fg%2F1hm3ryw9p!19sChIJPRRxa0FF0S0RFJJM0yZLrWw?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Krakatau Coffee &amp; Bakery</t>
+          <t>SMK PGRI Pesanggaran</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>4,3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dusun Kedaleman, Kemiren, Kec. Glagah, Kabupaten Banyuwangi, Jawa Timur 68432</t>
+          <t>C3MX+JQ9, Dusun Krajan, Pesanggaran, Kec. Pesanggaran, Kabupaten Banyuwangi, Jawa Timur 68488</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Krakatau+Coffee+%26+Bakery/data=!4m7!3m6!1s0x2dd14f79610ea3eb:0xa157badb48ae00a5!8m2!3d-8.2062175!4d114.326042!16s%2Fg%2F11srt084f7!19sChIJ66MOYXlP0S0RpQCuSNu6V6E?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+PGRI+Pesanggaran/data=!4m7!3m6!1s0x2dd4087f00363fcd:0x6275e28a3546ca13!8m2!3d-8.56597!4d114.0995!16s%2Fg%2F1hm3l015n!19sChIJzT82AH8I1C0RE8pGNYridWI?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Atap Langit Coffee</t>
+          <t>SMP Alam Banyuwangi Islamic School</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4,8</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Jl. MH.Tamrin, Pengantigan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68414</t>
+          <t>M524+4FJ, Dusun Kopen, Genteng Kulon, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Atap+Langit+Coffee/data=!4m7!3m6!1s0x2dd145237b71475d:0x487f0ebc631cac31!8m2!3d-8.2056284!4d114.3721771!16s%2Fg%2F11bzrp4k5j!19sChIJXUdxeyNF0S0RMawcY7wOf0g?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMP+Alam+Banyuwangi+Islamic+School/data=!4m7!3m6!1s0x2dd154d083d302fd:0x8e13d664b371131c!8m2!3d-8.3496714!4d114.1561375!16s%2Fg%2F11bxjlplp5!19sChIJ_QLTg9BU0S0RHBNxs2TWE44?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TMCE Taman Baru Coffee and Eatery</t>
+          <t>Banyuwangi</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Jl. Pajajaran, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>M4GX+R4M, Dusun Tegalyasan, Tegalarum, Kec. Sempu, Kabupaten Banyuwangi, Jawa Timur 68468</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/TMCE+Taman+Baru+Coffee+and+Eatery/data=!4m7!3m6!1s0x2dd15b33129be05d:0x8f4119a291f271d2!8m2!3d-8.2222547!4d114.3627452!16s%2Fg%2F11vy3_mwkw!19sChIJXeCbEjNb0S0R0nHykaIZQY8?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/Banyuwangi/data=!4m7!3m6!1s0x2dd155ce52277c2d:0xab728155b92e6d49!8m2!3d-8.322922!4d114.1478124!16s%2Fg%2F11q9k2t0vk!19sChIJLXwnUs5V0S0RSW0uuVWBcqs?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>53 Coffee and Eatery</t>
+          <t>SMP Negeri 3 Genteng</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Jl. Basuki Rahmat No.53, Singotrunan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68414</t>
+          <t>Jl. Kh. Kholil, Dusun Jalen 2 Desa No.1, Setail, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/53+Coffee+and+Eatery/data=!4m7!3m6!1s0x2dd145344435b2e9:0x640e0d61ddb61db2!8m2!3d-8.2032652!4d114.3739525!16s%2Fg%2F11rdgjhl14!19sChIJ6bI1RDRF0S0Rsh223WENDmQ?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMP+Negeri+3+Genteng/data=!4m7!3m6!1s0x2dd6ab351afd5c3d:0xb098ca85f39239bd!8m2!3d-8.3397211!4d114.1418834!16s%2Fg%2F1hm3hqhrx!19sChIJPVz9GjWr1i0RvTmS84XKmLA?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ujung Jawa Cafe &amp; Eatery</t>
+          <t>MTsN 8 Banyuwangi</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Jl. Mh Thamrin No.40, Singotrunan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68414</t>
+          <t>Jl. Samiran Dusun Krajan II.7, RT.003/RW.003, Jalen Parungan, Setail, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ujung+Jawa+Cafe+%26+Eatery/data=!4m7!3m6!1s0x2dd1453a40d03013:0x81062ddce592e3e0!8m2!3d-8.2055736!4d114.3718443!16s%2Fg%2F11v3hwzqts!19sChIJEzDQQDpF0S0R4OOS5dwtBoE?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/MTsN+8+Banyuwangi/data=!4m7!3m6!1s0x2dd6abe34bd4f447:0x6987da43e2793a09!8m2!3d-8.3647163!4d114.1413118!16s%2Fg%2F11shx1rpdb!19sChIJR_TUS-Or1i0RCTp54kPah2k?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Warung Èmboh Bakaran</t>
+          <t>SMA Negeri 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Jl. Adisucipto (utara patung kuda) karangente, Sobo, Banyuwangi Sub-District, Banyuwangi Regency, East Java 68418</t>
+          <t>Q9CC+MG6, Jl. Ikan Tongkol, Kertosari, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Warung+%C3%88mboh+Bakaran/data=!4m7!3m6!1s0x2dd15bf9e3358e35:0xbb6fe1a0f4feee0f!8m2!3d-8.2363857!4d114.3586367!16s%2Fg%2F11hxy7kb9p!19sChIJNY414_lb0S0RD-7-9KDhb7s?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Banyuwangi/data=!4m7!3m6!1s0x2dd15ad1ca1bb5d5:0x54c2a53169ee527a!8m2!3d-8.22833!4d114.3712772!16s%2Fg%2F121zcqkq!19sChIJ1bUbytFa0S0RelLuaTGlwlQ?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>DC Coffee Banyuwangi</t>
+          <t>SMA Negeri 1 Giri Banyuwangi</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4,7</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Jl. Sritanjung No.8, Temenggungan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68411</t>
+          <t>Jl. Hos. Cokroaminoto No.38, Dusun Watu Ulo, Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68425</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/DC+Coffee+Banyuwangi/data=!4m7!3m6!1s0x2dd145c5dc48c521:0x4b0ce4a7af9b9365!8m2!3d-8.2091422!4d114.3746964!16s%2Fg%2F11xrpmjkk1!19sChIJIcVI3MVF0S0RZZObr6fkDEs?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Giri+Banyuwangi/data=!4m7!3m6!1s0x2dd1454f7e84034f:0xf2d3ced3cdf38548!8m2!3d-8.2128646!4d114.3491807!16s%2Fg%2F1pxxn_c_4!19sChIJTwOEfk9F0S0RSIXzzdPO0_I?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SURYA KOPITIAM</t>
+          <t>SMA Muhammadiyah 2 Genteng</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Q9H7+Q7V, Taman Baru, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>J4QM+CCP, Jalen I, Setail, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/SURYA+KOPITIAM/data=!4m7!3m6!1s0x2dd15b1a9ed70e89:0xcf4855f709c8dc35!8m2!3d-8.2205096!4d114.3631858!16s%2Fg%2F11q8rprymb!19sChIJiQ7Xnhpb0S0RNdzICfdVSM8?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Muhammadiyah+2+Genteng/data=!4m7!3m6!1s0x2dd6ab2c2c18f9a9:0x8d75e66413ce55b7!8m2!3d-8.3612881!4d114.1334933!16s%2Fg%2F11scr52s7g!19sChIJqfkYLCyr1i0Rt1XOE2TmdY0?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>GARASI Kopi Roastery</t>
+          <t>MI Salafiyah 2 Setail</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Tk Rahmatullah, Jl. Mataram No.Utara, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68462</t>
+          <t>Jl. Ky. Ahmad No.20, Curahketangi Barat, Setail, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/GARASI+Kopi+Roastery/data=!4m7!3m6!1s0x2dd151133a82f4bd:0x83c713406ea2cded!8m2!3d-8.22576!4d114.3615319!16s%2Fg%2F11kkysf087!19sChIJvfSCOhNR0S0R7c2ibkATx4M?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/MI+Salafiyah+2+Setail/data=!4m7!3m6!1s0x2dd6ab30c3a05a93:0x245695cbedafea55!8m2!3d-8.343624!4d114.1341523!16s%2Fg%2F1hm1zrf8x!19sChIJk1qgwzCr1i0RVeqv7cuVViQ?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Kedai S.O ( Sogok Ontong Kopi)</t>
+          <t>SMP Ibrahimy Genteng</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Jl. MH.Tamrin No.19, Singotrunan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68423</t>
+          <t>Curahketangi Timur, Setail, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Kedai+S.O+%28+Sogok+Ontong+Kopi%29/data=!4m7!3m6!1s0x2dd145238655555b:0x8e964834dcfbf7d0!8m2!3d-8.2057471!4d114.3732685!16s%2Fg%2F11c612pmtk!19sChIJW1VVhiNF0S0R0Pf73DRIlo4?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMP+Ibrahimy+Genteng/data=!4m7!3m6!1s0x2dd6ab341d9e322d:0x500525dd6dd9d7ed!8m2!3d-8.34176!4d114.13807!16s%2Fg%2F1hm4g_g_h!19sChIJLTKeHTSr1i0R7dfZbd0lBVA?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Moxie Coffee and Eatery</t>
+          <t>SMP Negeri 1 Genteng</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Q9J3+267, Jl. Brawijaya, Lingkungan Cuking Rw., Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68425</t>
+          <t>Jl. Bromo No.49, Dusun Krajan, Genteng Kulon, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Moxie+Coffee+and+Eatery/data=!4m7!3m6!1s0x2dd145a9e45c8989:0x9b543153ced4e2eb!8m2!3d-8.2199519!4d114.3530562!16s%2Fg%2F11gl0jvrpc!19sChIJiYlc5KlF0S0R6-LUzlMxVJs?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMP+Negeri+1+Genteng/data=!4m7!3m6!1s0x2dd1552ba21d504d:0xda64ce5c2f73047e!8m2!3d-8.3609185!4d114.1471492!16s%2Fg%2F1hm3f42x6!19sChIJTVAdoitV0S0RfgRzL1zOZNo?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Albirru Coffee and Eatery</t>
+          <t>MAN 2 BANYUWANGI</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Dusun Watu Ulo, Rejosari, Kec. Glagah, Kabupaten Banyuwangi, Jawa Timur</t>
+          <t>JL Kyai Haji Wachid Hasyim No.06, Dusun Kopen, Genteng Kulon, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Albirru+Coffee+and+Eatery/data=!4m7!3m6!1s0x2dd1450a93378bb7:0xe407efcb4c85fd3b!8m2!3d-8.2129285!4d114.3480762!16s%2Fg%2F11mk70_2bs!19sChIJt4s3kwpF0S0RO_2FTMvvB-Q?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/MAN+2+BANYUWANGI/data=!4m7!3m6!1s0x2dd154d30135f8e3:0x36544cfac37054!8m2!3d-8.349737!4d114.14667!16s%2Fg%2F1hm379yvc!19sChIJ4_g1AdNU0S0RVHDD-kxUNgA?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Palm Sugar Cafe</t>
+          <t>SMA Negeri 1 Genteng</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Jl. Kuntulan No.135, Lingkungan Karang Ase, Bakungan, Kec. Glagah, Kabupaten Banyuwangi, Jawa Timur 68431</t>
+          <t>J4WW+WHW, Jl. KH. Wahid Hasyim No.20, Dusun Kopen, Genteng Kulon, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Palm+Sugar+Cafe/data=!4m7!3m6!1s0x2dd145518d994c01:0x4780bec5a8e4dd72!8m2!3d-8.2172771!4d114.3442171!16s%2Fg%2F11gd67hd8l!19sChIJAUyZjVFF0S0Rct3kqMW-gEc?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Genteng/data=!4m7!3m6!1s0x2dd154d48c5629f9:0x4f8ad785c82e3d4a!8m2!3d-8.3531617!4d114.1457066!16s%2Fg%2F12dpx4yz7!19sChIJ-SlWjNRU0S0RSj0uyIXXik8?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Omah Majapahit Cafe &amp; Resto</t>
+          <t>MAN 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Jl. Singosari No.33, Taman Baru, Banyuwangi Kota, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Ikan Tengiri No.02, Sobo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Omah+Majapahit+Cafe+%26+Resto/data=!4m7!3m6!1s0x2dd15b1b64439fbf:0x7de4b96e25a6a211!8m2!3d-8.2266805!4d114.3622604!16s%2Fg%2F11rhf80mym!19sChIJv59DZBtb0S0REaKmJW655H0?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/MAN+1+Banyuwangi/data=!4m7!3m6!1s0x2dd15ac61723f3f1:0x67bb2fcda2ba3800!8m2!3d-8.2326999!4d114.3626654!16s%2Fg%2F1225qd9h!19sChIJ8fMjF8Za0S0RADi6os0vu2c?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>kopi jotos</t>
+          <t>BRINDO INTERNATIONAL SCHOOL BANYUWANGI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Jl. Panglima Besar Sudirman No.33, Penganjuran, Panderejo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68415</t>
+          <t>Jl. Mendut Regency No.D-15, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/kopi+jotos/data=!4m7!3m6!1s0x2dd1452d6d15a447:0x4171b695db29d8c2!8m2!3d-8.214574!4d114.3706726!16s%2Fg%2F11hwxxn8r_!19sChIJR6QVbS1F0S0Rwtgp25W2cUE?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/BRINDO+INTERNATIONAL+SCHOOL+BANYUWANGI/data=!4m7!3m6!1s0x2dd1456fb2b02889:0xc1678df0fc362ec2!8m2!3d-8.2196248!4d114.3624716!16s%2Fg%2F11rwpch528!19sChIJiSiwsm9F0S0Rwi42_PCNZ8E?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Amethyst Kopi Banyuwangi</t>
+          <t>SMA Negeri 1 Rogojampi</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Jl. Kepiting No.100, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
+          <t>Jl. Ali Sakti No. 2, Pengantigan, Rogojampi, Guri, Pengatigan, Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68462</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Amethyst+Kopi+Banyuwangi/data=!4m7!3m6!1s0x2dd15b00410e502f:0x615f2675534a012e!8m2!3d-8.2329134!4d114.3647793!16s%2Fg%2F11w7kl63s7!19sChIJL1AOQQBb0S0RLgFKU3UmX2E?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Rogojampi/data=!4m7!3m6!1s0x2dd150d433f3b38f:0xe926952ad5c4b609!8m2!3d-8.3037194!4d114.2901773!16s%2Fg%2F12dpwl3b8!19sChIJj7PzM9RQ0S0RCbbE1SqVJuk?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>TILU</t>
+          <t>SMA Negeri 1 Bangorejo</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4,6</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Jl. Kolonel Sugiono No.2a, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Bhayangkara No.10, Kebonrejo, Kebondalem, Kec. Bangorejo, Kabupaten Banyuwangi, Jawa Timur 68487</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/TILU/data=!4m7!3m6!1s0x2dd15bdb4ab61ee1:0x320dff0bd0b1b68e!8m2!3d-8.2270161!4d114.3699137!16s%2Fg%2F11jrcqrg66!19sChIJ4R62Sttb0S0Rjrax0Av_DTI?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Bangorejo/data=!4m7!3m6!1s0x2dd40756848e5511:0xcfc22423d6ca4b06!8m2!3d-8.4854454!4d114.1403602!16s%2Fg%2F11b6g6bn77!19sChIJEVWOhFYH1C0RBkvK1iMkws8?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Hedon Estate Banyuwangi | Cafe &amp; Resto</t>
+          <t>SMA NEGERI 1 GAMBIRAN</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Jl. Gajah Mada Lingkungan Mojoroto Rumah Panggung, Lingkungan Mojoroto R, Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68422</t>
+          <t>H57C+VC4, Sumberjaya, Wringin Agung, Kec. Gambiran, Kabupaten Banyuwangi, Jawa Timur 68486</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Hedon+Estate+Banyuwangi+%7C+Cafe+%26+Resto/data=!4m7!3m6!1s0x2dd145a9d31987e7:0x8b5a16a29e8e6ae2!8m2!3d-8.2082507!4d114.3562904!16s%2Fg%2F11j0c9njl4!19sChIJ54cZ06lF0S0R4mqOnqIWWos?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+NEGERI+1+GAMBIRAN/data=!4m7!3m6!1s0x2dd3ff36a081f53f:0xa937336fe32e46aa!8m2!3d-8.4357069!4d114.1705133!16s%2Fg%2F11c5rt_jtq!19sChIJP_WBoDb_0y0RqkYu428zN6k?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Osing Deles Cafe &amp; Resto</t>
+          <t>SMA Negeri 1 Glenmore</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Jl. K.H. Agus Salim No.12A, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>P24J+47M, Jl. RS Bakti Husada Krikilan, Glenmore, Dusun Krajan, Tegalharjo, Kec. Glenmore, Kabupaten Banyuwangi, Jawa Timur 68466</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Osing+Deles+Cafe+%26+Resto/data=!4m7!3m6!1s0x2dd15b58585dff81:0x83ed30e42c2a615d!8m2!3d-8.2284476!4d114.3617203!16s%2Fg%2F11g0m4vlb5!19sChIJgf9dWFhb0S0RXWEqLOQw7YM?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Glenmore/data=!4m7!3m6!1s0x2dd6ae921ec6597d:0x5ea59c4104658ee3!8m2!3d-8.294657!4d114.0306861!16s%2Fg%2F11c5r_d3f7!19sChIJfVnGHpKu1i0R445lBEGcpV4?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Kemunir Kopi</t>
+          <t>SMA Negeri 1 Pesanggaran</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Jl. Penataran No.49, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>C3VP+8XP, Mulyosari, Sumbermulyo, Kec. Pesanggaran, Kabupaten Banyuwangi, Jawa Timur 68488</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Kemunir+Kopi/data=!4m7!3m6!1s0x2dd14533a843e4af:0x99a4eb1f2bdfc1c3!8m2!3d-8.2189357!4d114.366237!16s%2Fg%2F11cn3m1k8r!19sChIJr-RDqDNF0S0Rw8HfKx_rpJk?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Pesanggaran/data=!4m7!3m6!1s0x2dd407d473263b4b:0xaa322fa78951d749!8m2!3d-8.5585304!4d114.1008702!16s%2Fg%2F11csqgxsvm!19sChIJSzsmc9QH1C0RSddRiacvMqo?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Indische 1931 Banyuwangi</t>
+          <t>SMA MUHAMMADIYAH 1 BANYUWANGI</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Q9F7+23P, Simpang, Jl. Singosari, Taman Baru, Banyuwangi Sub-District, Banyuwangi Regency, East Java 68416</t>
+          <t>Q9H2+G6P, Lingkungan Watu Ulo R, Bakungan, Kec. Glagah, Kabupaten Banyuwangi, Jawa Timur 68431</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Indische+1931+Banyuwangi/data=!4m7!3m6!1s0x2dd15bf3cd423831:0xc2da49d291492f53!8m2!3d-8.2274114!4d114.36271!16s%2Fg%2F11n8zvwqb9!19sChIJMThCzfNb0S0RUy9JkdJJ2sI?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+MUHAMMADIYAH+1+BANYUWANGI/data=!4m7!3m6!1s0x2dd145051839debf:0xd5de92f0640cd5e1!8m2!3d-8.2211526!4d114.3505745!16s%2Fg%2F11sc00c3mv!19sChIJv945GAVF0S0R4dUMZPCS3tU?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Dominance Coffee</t>
+          <t>SMA Negeri 1 Tegaldlimo</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Jl. Kertanegara No.10 A, Kebalenan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68417</t>
+          <t>Jl. Wijaya Kusuma No.1, Bayatrejo, Wringinpitu, Kec. Tegaldlimo, Kabupaten Banyuwangi, Jawa Timur 56172</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Dominance+Coffee/data=!4m7!3m6!1s0x2dd15bee4d0fb1a3:0x88b6a435d050ed1e!8m2!3d-8.2313925!4d114.3543418!16s%2Fg%2F11pq4jrsz2!19sChIJo7EPTe5b0S0RHu1Q0DWktog?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Tegaldlimo/data=!4m7!3m6!1s0x2dd145259a829f79:0x9dc74be6b9281af4!8m2!3d-8.4957678!4d114.2813831!16s%2Fg%2F11c5rvzkhw!19sChIJeZ-CmiVF0S0R9BooueZLx50?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>RIHAT Toko Kopi</t>
+          <t>SMA Negeri 1 Muncar</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Kepatihan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur</t>
+          <t>Jalan Sraten - Tapanrejo No.1, RT.03/RW.06, Dusun Kedung Dandang, Tapanrejo, Kec. Muncar, Kabupaten Banyuwangi, Jawa Timur 68472</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/RIHAT+Toko+Kopi/data=!4m7!3m6!1s0x2dd1452450843bdb:0xafcba21dea79aee0!8m2!3d-8.2132656!4d114.3756778!16s%2Fg%2F11sfvnq225!19sChIJ2zuEUCRF0S0R4K556h2iy68?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Muncar/data=!4m7!3m6!1s0x2dd3fcc1b3ea7315:0xcc737d624b188eb5!8m2!3d-8.4449804!4d114.3124433!16s%2Fg%2F11c5rv26ht!19sChIJFXPqs8H80y0RtY4YS2J9c8w?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Jajung Cafe</t>
+          <t>SMA 17 Agustus 1945 Banyuwangi</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Jl. Stasiun Karangasem, Lingkungan Karang Asem, Bakungan, Kec. Glagah, Kabupaten Banyuwangi, Jawa Timur 68431</t>
+          <t>Jl. Jember Kalibaru-Banyuwangi No.31, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Jajung+Cafe/data=!4m7!3m6!1s0x2dd15b0df46d9c6f:0xd0acf774acd49a3f!8m2!3d-8.2239822!4d114.3407005!16s%2Fg%2F11fnsbr183!19sChIJb5xt9A1b0S0RP5rUrHT3rNA?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+17+Agustus+1945+Banyuwangi/data=!4m7!3m6!1s0x2dd15b5068ee7981:0xc60ecacaffa4ad6a!8m2!3d-8.2523626!4d114.342917!16s%2Fg%2F11gy69zj49!19sChIJgXnuaFBb0S0Raq2k_8rKDsY?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Sukaria Foodpark</t>
+          <t>SD Muhammadiyah 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Jl. KH. Wahid Hasyim No.45, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Jaksa Agung Suprapto No.60, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Sukaria+Foodpark/data=!4m7!3m6!1s0x2dd145ec365d79bd:0x13559a4205152642!8m2!3d-8.2162966!4d114.3724679!16s%2Fg%2F11sd88l8j0!19sChIJvXldNuxF0S0RQiYVBUKaVRM?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SD+Muhammadiyah+1+Banyuwangi/data=!4m7!3m6!1s0x2dd14533df4d743b:0x6aa6daec2cdc3327!8m2!3d-8.2162737!4d114.3635719!16s%2Fg%2F1pzxnsqdf!19sChIJO3RN3zNF0S0RJzPcLOzapmo?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Toko Kopi Singgasana</t>
+          <t>SMA Lb PGRI Banyuwangi</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Di depan singgasana lama, Gg. Kenanga V, Singonegaran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68415</t>
+          <t>Jl. Tunggul Ametung Gg. III No.52, Kebalenan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68417</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Toko+Kopi+Singgasana/data=!4m7!3m6!1s0x2dd145e50cf369ab:0x8269d5b0ae266846!8m2!3d-8.2110787!4d114.363283!16s%2Fg%2F11lh4x08c0!19sChIJq2nzDOVF0S0RRmgmrrDVaYI?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Lb+PGRI+Banyuwangi/data=!4m7!3m6!1s0x2dd15ab805528443:0xdf21d4daff7f885d!8m2!3d-8.2327874!4d114.3572847!16s%2Fg%2F1hm50_nbx!19sChIJQ4RSBbha0S0RXYh__9rUId8?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Umarasa cafe &amp; Resto</t>
+          <t>SMA Negeri 1 Srono</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4,5</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Jl. Adi Sucipto No.44, Sobo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
+          <t>J7HR+9JG, Unnamed Rd, Krajan Baru, Kebaman, Kec. Srono, Kabupaten Banyuwangi, Jawa Timur 68471</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Umarasa+cafe+%26+Resto/data=!4m7!3m6!1s0x2dd15b21b7c49d5d:0x9d0e545243b83d2b!8m2!3d-8.230437!4d114.363295!16s%2Fg%2F11pcn8152m!19sChIJXZ3EtyFb0S0RKz24Q1JUDp0?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+1+Srono/data=!4m7!3m6!1s0x2dd157cbc47b1f39:0x834da5c809e9bce1!8m2!3d-8.371566!4d114.2915802!16s%2Fg%2F11csqfl1t1!19sChIJOR97xMtX0S0R4bzpCcilTYM?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Kopi Pinarak Banyuwangi</t>
+          <t>SMK AL FIRDAUS</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Jl. Kepiting No.77 Lantai 2, Tukangkayu, Banyuwangi Sub-District, Banyuwangi Regency, East Java 68418</t>
+          <t>Dusun Panjen, Tlogosari, Jambewangi, Kec. Sempu, Kabupaten Banyuwangi, Jawa Timur 68468</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Kopi+Pinarak+Banyuwangi/data=!4m7!3m6!1s0x2dd15bd423f0d607:0x55cd936cab24d10f!8m2!3d-8.233358!4d114.3643393!16s%2Fg%2F11qqffz_8d!19sChIJB9bwI9Rb0S0RD9Ekq2yTzVU?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMK+AL+FIRDAUS/data=!4m7!3m6!1s0x2dd6ad5dced42a6d:0xf94ecb0f87a22f3b!8m2!3d-8.298109!4d114.1293177!16s%2Fg%2F11xz7n682w!19sChIJbSrUzl2t1i0ROy-ihw_LTvk?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Ngelaxx Cafe</t>
+          <t>SMP Negeri 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Jl. Jaksa Agung Suprapto No.74, Lingkungan Cuking Rw., Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Jenderal Ahmad Yani No.74, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Ngelaxx+Cafe/data=!4m7!3m6!1s0x2dd14549e7f92b17:0xd1c501e1e0a53c67!8m2!3d-8.2159119!4d114.357207!16s%2Fg%2F11g727rt_c!19sChIJFyv550lF0S0RZzyl4OEBxdE?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMP+Negeri+1+Banyuwangi/data=!4m7!3m6!1s0x2dd14532bfbe6515:0xb3472fcba0712b19!8m2!3d-8.220484!4d114.368491!16s%2Fg%2F121j1z6m!19sChIJFWW-vzJF0S0RGStxoMsvR7M?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Deli Bakery ,Resto &amp; Gallery</t>
+          <t>SD Negeri Kepatihan Banyuwangi</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Jl. Jenderal Ahmad Yani No.68, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Q9QG+FVX, Kepatihan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68411</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Deli+Bakery+,Resto+%26+Gallery/data=!4m7!3m6!1s0x2dd145dcdf3ea1f9:0x8bdd23ae7822f54!8m2!3d-8.2196736!4d114.3687241!16s%2Fg%2F11ks9rq6ph!19sChIJ-aE-39xF0S0RVC-C5zrSvQg?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SD+Negeri+Kepatihan+Banyuwangi/data=!4m7!3m6!1s0x2dd1452897721649:0x6e6c9aafa2017caf!8m2!3d-8.2112663!4d114.3772472!16s%2Fg%2F1hm2sh_v3!19sChIJSRZylyhF0S0Rr3wBoq-abG4?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Padi's coffe and Eatery</t>
+          <t>SMA Negeri 2 Taruna Bhayangkara</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Jl. Mendut Gg. 5, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Pandan, Pandan, Kembiritan, Kec. Genteng, Kabupaten Banyuwangi, Jawa Timur 68465</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Padi%27s+coffe+and+Eatery/data=!4m7!3m6!1s0x2dd1457d5abfacd7:0xdbb581ade9d60fbd!8m2!3d-8.2205736!4d114.3634893!16s%2Fg%2F11ldpc947q!19sChIJ16y_Wn1F0S0RvQ_W6a2Btds?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMA+Negeri+2+Taruna+Bhayangkara/data=!4m7!3m6!1s0x2dd155a725d2a9bb:0xbc3ec3f0b365c083!8m2!3d-8.3683874!4d114.1951834!16s%2Fg%2F1q5bl8c4w!19sChIJu6nSJadV0S0Rg8Bls_DDPrw?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Toko Kopi Tetangga 2.0</t>
+          <t>SMAN 1 Wongsorejo</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Sobo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
+          <t>XC78+RMM, Krajan, Bengkak, Kec. Wongsorejo, Kabupaten Banyuwangi, Jawa Timur 68453</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Toko+Kopi+Tetangga+2.0/data=!4m7!3m6!1s0x2dd15ba3488b2b4f:0x493b1e9cab2f74f4!8m2!3d-8.2357349!4d114.3618406!16s%2Fg%2F11r_mhd5qt!19sChIJTyuLSKNb0S0R9HQvq5weO0k?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMAN+1+Wongsorejo/data=!4m7!3m6!1s0x2dd138c7e71742ef:0x6a8ee19dec823d56!8m2!3d-8.0354048!4d114.4166761!16s%2Fg%2F11csqh_tp7!19sChIJ70IX58c40S0RVj2C7J3hjmo?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Conato Cafe Bakery</t>
+          <t>SD Katholik Santa Maria</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4,4</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Depan Roxy Mall, Jl. Jenderal Ahmad Yani No.21-23, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Jaksa Agung Suprapto No.84, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Conato+Cafe+Bakery/data=!4m7!3m6!1s0x2dd14532c9b5f4d1:0x3b2f6721e76fea34!8m2!3d-8.2174438!4d114.3694839!16s%2Fg%2F1pzyj2kvw!19sChIJ0fS1yTJF0S0RNOpv5yFnLzs?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SD+Katholik+Santa+Maria/data=!4m7!3m6!1s0x2dd145368039d511:0x393a7b84d45799fe!8m2!3d-8.2165297!4d114.3609395!16s%2Fg%2F11c47mytry!19sChIJEdU5gDZF0S0R_plX1IR7Ojk?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Tamulang Co-Working Space and Cafe</t>
+          <t>SMP Negeri 2 Banyuwangi</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Q9G6+29C, Taman Baru, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Rangga Wuni No.41, Kebalenan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68417</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Tamulang+Co-Working+Space+and+Cafe/data=!4m7!3m6!1s0x2dd15b3f114fb1b3:0x7a776a5a45ebf68a!8m2!3d-8.2249271!4d114.3608891!16s%2Fg%2F11gvrv4f1h!19sChIJs7FPET9b0S0RivbrRVpqd3o?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMP+Negeri+2+Banyuwangi/data=!4m7!3m6!1s0x2dd15ab62597bb4d:0x2b7875bf9078d899!8m2!3d-8.2288256!4d114.3573824!16s%2Fg%2F1hm278kbw!19sChIJTbuXJbZa0S0Rmdh4kL91eCs?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Kembang langit Traditional Restoran &amp; cafe</t>
+          <t>SMAK Hikmah Mandala</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Jl. Kepiting No.80a, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Jaksa Agung Suprapto No.74, Penganjuran, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Kembang+langit+Traditional+Restoran+%26+cafe/data=!4m7!3m6!1s0x2dd15b977b0ff85b:0xe1ae9f021a6d1748!8m2!3d-8.2334292!4d114.3642248!16s%2Fg%2F11s5gvvvkt!19sChIJW_gPe5db0S0RSBdtGgKfruE?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMAK+Hikmah+Mandala/data=!4m7!3m6!1s0x2dd14536ac727c99:0xfd168b7daf055c4c!8m2!3d-8.2166029!4d114.361232!16s%2Fg%2F1pzrlzlmn!19sChIJmXxyrDZF0S0RTFwFr32LFv0?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>NOGI Coffee &amp; Space</t>
+          <t>SMPN 1 Giri</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Jl. Letjen Sutoyo No.21, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68416</t>
+          <t>Jl. Wijaya Kusuma No.103, Lingkungan Cuking Rw., Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68425</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/NOGI+Coffee+%26+Space/data=!4m7!3m6!1s0x2dd14500692f1ab9:0x8371b694f054b4e4!8m2!3d-8.220956!4d114.3714878!16s%2Fg%2F11xcwl4z5h!19sChIJuRovaQBF0S0R5LRU8JS2cYM?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SMPN+1+Giri/data=!4m7!3m6!1s0x2dd145443bf75c6f:0xe36666f5e3053432!8m2!3d-8.2088966!4d114.3507055!16s%2Fg%2F1hm31ctw3!19sChIJb1z3O0RF0S0RMjQF4_VmZuM?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Java Sunrise Cafe</t>
+          <t>MTs Negeri 1 Banyuwangi</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Jl. MH.Tamrin No.217, Pengantigan, Giri, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68423</t>
+          <t>Jl. Mawar No.35, Lingkungan Mojoroto R, Mojopanggung, Kec. Giri, Kabupaten Banyuwangi, Jawa Timur 68422</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/Java+Sunrise+Cafe/data=!4m7!3m6!1s0x2dd1453e189eddb9:0xdd320c1733a9e664!8m2!3d-8.2020535!4d114.3623377!16s%2Fg%2F11bcf047h9!19sChIJud2eGD5F0S0RZOapMxcMMt0?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/MTs+Negeri+1+Banyuwangi/data=!4m7!3m6!1s0x2dd145576b7d8b67:0x1fa3ff175b4d8907!8m2!3d-8.2065963!4d114.3551395!16s%2Fg%2F11hz01p4ll!19sChIJZ4t9a1dF0S0RB4lNWxf_ox8?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>La Costa Cafe and Restaurant</t>
+          <t>SD NEGERI MODEL BANYUWANGI</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4,3</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Jl. Piere Tendean No.89, Karangrejo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68411</t>
+          <t>Jl. Ikan Wijinongko No.23, Sobo, Tukangkayu, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68418</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://www.google.com/maps/place/La+Costa+Cafe+and+Restaurant/data=!4m7!3m6!1s0x2dd1452c0d9e1b53:0xfb38e1a36972fc43!8m2!3d-8.217086!4d114.3751644!16s%2Fg%2F11gdzrkclb!19sChIJUxueDSxF0S0RQ_xyaaPhOPs?authuser=0&amp;hl=id&amp;rclk=1</t>
+          <t>https://www.google.com/maps/place/SD+NEGERI+MODEL+BANYUWANGI/data=!4m7!3m6!1s0x2dd15b4784c4ccd1:0xc59a34bb41411432!8m2!3d-8.2364923!4d114.36903!16s%2Fg%2F11sg3xdyg4!19sChIJ0czEhEdb0S0RMhRBQbs0msU?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>MI Roudlotul Ulum Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Q9Q9+8FH, Jl. Bengawan, Panderejo, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68415</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MI+Roudlotul+Ulum+Banyuwangi/data=!4m7!3m6!1s0x2dd14505865afc61:0x4764e7f1cd2169dd!8m2!3d-8.2116916!4d114.3687242!16s%2Fg%2F11fvg_hskd!19sChIJYfxahgVF0S0R3WkhzfHnZEc?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>MATIQ AL-USWAH BANYUWANGI</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Q88R+M28, Jl. Cemara, Dusun Krajan, Kebalenan, Kec. Glagah, Kabupaten Banyuwangi, Jawa Timur 68432</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MATIQ+AL-USWAH+BANYUWANGI/data=!4m7!3m6!1s0x2dd15b970ec52eb1:0x2ad084d87c04f7a6!8m2!3d-8.2333274!4d114.3400819!16s%2Fg%2F11q2q137rg!19sChIJsS7FDpdb0S0RpvcEfNiE0Co?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>SD Bloom Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>RT.01/RW.2 Jatisari, Dusun Krajan I, Wringin Agung, Kec. Gambiran, Kabupaten Banyuwangi, Jawa Timur 68486</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SD+Bloom+Banyuwangi/data=!4m7!3m6!1s0x2dd155552554ae23:0x95df804c76c8d534!8m2!3d-8.4341452!4d114.1785703!16s%2Fg%2F11l44rjtk2!19sChIJI65UJVVV0S0RNNXIdkyA35U?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Sekolah Menengah Atas Favorit Tegal Dlimo</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Q9QF+VCR, JL. Gempol Dampit, Kepatihan, Kec. Banyuwangi, Kabupaten Banyuwangi, Jawa Timur 68411</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+Menengah+Atas+Favorit+Tegal+Dlimo/data=!4m7!3m6!1s0x2dd145259a829f79:0x68de59288f4b62cc!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F1pztywt17!19sChIJeZ-CmiVF0S0RzGJLjyhZ3mg?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Gd</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Gd/data=!4m7!3m6!1s0x2dd1452533909ad7:0x19d997927b69d91f!8m2!3d-8.2095315!4d114.3701297!16s%2Fg%2F1hm44g7t_!19sChIJ15qQMyVF0S0RH9lpe5KX2Rk?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SD Al Irsyad Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SD+Al+Irsyad+Banyuwangi/data=!4m7!3m6!1s0x2dd145220d6b230b:0x4401fae9759709c6!8m2!3d-8.2014868!4d114.3743474!16s%2Fg%2F11b76cg3r2!19sChIJCyNrDSJF0S0RxgmXden6AUQ?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>MIN 1 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MIN+1+Banyuwangi/data=!4m7!3m6!1s0x2dd15ac5d348c7cd:0x3a8d6689f355d956!8m2!3d-8.2342545!4d114.3645128!16s%2Fg%2F11c5558fj5!19sChIJzcdI08Va0S0RVtlV84lmjTo?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>The Saba School</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/The+Saba+School/data=!4m7!3m6!1s0x2dd1452fe655e247:0x6a6b1290d182a53d!8m2!3d-8.2124946!4d114.3707951!16s%2Fg%2F11c52xy3kb!19sChIJR-JV5i9F0S0RPaWC0ZASa2o?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SMK PGRI Rogojampi</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMK+PGRI+Rogojampi/data=!4m7!3m6!1s0x2dd15746b66162bb:0xe6bf78c2db9e010c!8m2!3d-8.3025401!4d114.2950229!16s%2Fg%2F1hm41qzwq!19sChIJu2JhtkZX0S0RDAGe28J4v-Y?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>TK Negeri Model</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TK+Negeri+Model/data=!4m7!3m6!1s0x2dd15ac43680a0dd:0x8e3da838ea193040!8m2!3d-8.2368393!4d114.3694534!16s%2Fg%2F1pzsnc2mz!19sChIJ3aCANsRa0S0RQDAZ6jioPY4?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Sekolah Menengah Atas NU Genteng</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+Menengah+Atas+NU+Genteng/data=!4m7!3m6!1s0x2dd145259a829f79:0x244b0d7f7429d3e1!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F1pzx4nrxm!19sChIJeZ-CmiVF0S0R4dMpdH8NSyQ?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>SMP Negeri 5 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Negeri+5+Banyuwangi/data=!4m7!3m6!1s0x2dd14536a40cb635:0x1411ea1a193bfbd9!8m2!3d-8.2163087!4d114.362775!16s%2Fg%2F1hm52pc2v!19sChIJNbYMpDZF0S0R2fs7GRrqERQ?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Sekolah GRETA (SD-SMP)</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+GRETA+%28SD-SMP%29/data=!4m7!3m6!1s0x2dd3ff9d9c8fc0af:0xf3a65f6b2ae9d339!8m2!3d-8.441159!4d114.1900931!16s%2Fg%2F11f7dpgv_4!19sChIJr8CPnJ3_0y0ROdPpKmtfpvM?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SMPIT AL USWAH BANYUWANGI</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMPIT+AL+USWAH+BANYUWANGI/data=!4m7!3m6!1s0x2dd15aa5f8ce7361:0x686622e37b252594!8m2!3d-8.2331144!4d114.3403657!16s%2Fg%2F11c14t09fq!19sChIJYXPO-KVa0S0RlCUle-MiZmg?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SMALB negeri Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMALB+negeri+Banyuwangi/data=!4m7!3m6!1s0x2dd14545c7618147:0xfffa19f1ac1a0c60!8m2!3d-8.2111499!4d114.3504125!16s%2Fg%2F11gbxd07l_!19sChIJR4Fhx0VF0S0RYAwarPEZ-v8?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Sekolah Menengah Atas PGRI Purwoharjo</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+Menengah+Atas+PGRI+Purwoharjo/data=!4m7!3m6!1s0x2dd145259a829f79:0x68bcad40db0b9b90!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F1pzq5r6py!19sChIJeZ-CmiVF0S0RkJsL20CtvGg?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Sekolah Kapal Pesiar Blambangan College</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+Kapal+Pesiar+Blambangan+College/data=!4m7!3m6!1s0x2dd15bda39f6c703:0x4d2df1a0b199595e!8m2!3d-8.2341467!4d114.3683814!16s%2Fg%2F11nrw351gj!19sChIJA8f2Odpb0S0RXlmZsaDxLU0?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Kantor Neutron Yogyakarta Cabang Banyuwangi-1</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Kantor+Neutron+Yogyakarta+Cabang+Banyuwangi-1/data=!4m7!3m6!1s0x2dd14548f8786147:0x851844dcfb38b66b!8m2!3d-8.2142591!4d114.3548889!16s%2Fg%2F11fxvwf79b!19sChIJR2F4-EhF0S0Ra7Y4-9xEGIU?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SMP Negeri 3 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Negeri+3+Banyuwangi/data=!4m7!3m6!1s0x2dd1451711a4240f:0x8d992793eaa0b0db!8m2!3d-8.1979402!4d114.3677764!16s%2Fg%2F12vs2pm_w!19sChIJDySkERdF0S0R27Cg6pMnmY0?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Magistra Utama Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Magistra+Utama+Banyuwangi/data=!4m7!3m6!1s0x2dd1453b1923e071:0x2169266c80cbc64b!8m2!3d-8.2322473!4d114.3614197!16s%2Fg%2F1pzr5_q53!19sChIJceAjGTtF0S0RS8bLgGwmaSE?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SD Islam Terpadu Al Uswah 2</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SD+Islam+Terpadu+Al+Uswah+2/data=!4m7!3m6!1s0x2dd15aaf5688b9ad:0x33f3262bc39ae97b!8m2!3d-8.2334651!4d114.3402028!16s%2Fg%2F11cls6nnk9!19sChIJrbmIVq9a0S0Re-mawysm8zM?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>MTs Darunnajah</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MTs+Darunnajah/data=!4m7!3m6!1s0x2dd1452d036d2acf:0x74917f4433ea107!8m2!3d-8.2188805!4d114.3730252!16s%2Fg%2F1hm2b0fv_!19sChIJzyptAy1F0S0RB6E-Q_QXSQc?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Universitas PGRI Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Universitas+PGRI+Banyuwangi/data=!4m7!3m6!1s0x2dd14532ca02e0f1:0x8716e849141a95f9!8m2!3d-8.2275505!4d114.3721847!16s%2Fg%2F12qhknf_f!19sChIJ8eACyjJF0S0R-ZUaFEnoFoc?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>SMP Katolik Santo Yusup Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Katolik+Santo+Yusup+Banyuwangi/data=!4m7!3m6!1s0x2dd145315245ae1d:0xfe3aacc27b3aafc7!8m2!3d-8.216267!4d114.364327!16s%2Fg%2F1hm5rl9c3!19sChIJHa5FUjFF0S0Rx686e8KsOv4?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>SMP Negeri 1 Glagah Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Negeri+1+Glagah+Banyuwangi/data=!4m7!3m6!1s0x2dd14544531c8005:0xbe71306c1f8e4542!8m2!3d-8.2097585!4d114.3495544!16s%2Fg%2F11fxzm5xls!19sChIJBYAcU0RF0S0RQkWOH2wwcb4?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>SDN Kebalenan</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SDN+Kebalenan/data=!4m7!3m6!1s0x2dd15ac817b13ca1:0x96286affb101c85b!8m2!3d-8.2310677!4d114.3588848!16s%2Fg%2F1hm4j672c!19sChIJoTyxF8ha0S0RW8gBsf9qKJY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>SDIT AL USWAH BANYUWANGI</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SDIT+AL+USWAH+BANYUWANGI/data=!4m7!3m6!1s0x2dd14505aeeacfeb:0xb879d75628459cee!8m2!3d-8.1879201!4d114.3723009!16s%2Fg%2F11c1wgxht1!19sChIJ68_qrgVF0S0R7pxFKFbXebg?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Cabang Dinas Pendidikan Provinsi Jawa Timur Kabupaten Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Cabang+Dinas+Pendidikan+Provinsi+Jawa+Timur+Kabupaten+Banyuwangi/data=!4m7!3m6!1s0x2dd145223530627d:0x193fb6fe567e7823!8m2!3d-8.203344!4d114.3744115!16s%2Fg%2F11dxbcxrsc!19sChIJfWIwNSJF0S0RI3h-Vv62Pxk?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>SMA Negeri 2 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMA+Negeri+2+Banyuwangi/data=!4m7!3m6!1s0x2dd145fd15906507:0xe3622ff896e99205!8m2!3d-8.2128825!4d114.3499606!16s%2Fg%2F11tn6rnj1z!19sChIJB2WQFf1F0S0RBZLplvgvYuM?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>KB-TK Taman Quran Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/KB-TK+Taman+Quran+Banyuwangi/data=!4m7!3m6!1s0x2dd15ab749847b7f:0x736c2fe6b771e923!8m2!3d-8.2313125!4d114.3525625!16s%2Fg%2F11f1241bdf!19sChIJf3uESbda0S0RI-lxt-YvbHM?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Pondok Pesantren Adz Dzikra &amp; Masjid Al Ahwa Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Pondok+Pesantren+Adz+Dzikra+%26+Masjid+Al+Ahwa+Banyuwangi/data=!4m7!3m6!1s0x2dd15b8a42c0e267:0xc1f02c15b683340b!8m2!3d-8.2299959!4d114.3671358!16s%2Fg%2F11jgmcl0wx!19sChIJZ-LAQopb0S0RCzSDthUs8ME?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Sdlb Matahati Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sdlb+Matahati+Banyuwangi/data=!4m7!3m6!1s0x2dd15b43ccf50e4d:0x274243f09c832d3!8m2!3d-8.2340208!4d114.3483132!16s%2Fg%2F11gygzgrvq!19sChIJTQ71zENb0S0R0zLICT8kdAI?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>TK DaQu School Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TK+DaQu+School+Banyuwangi/data=!4m7!3m6!1s0x2dd15ab9ee6aeb11:0x4897cdccaab963ac!8m2!3d-8.2276044!4d114.34983!16s%2Fg%2F11g6rdgwhb!19sChIJEetq7rla0S0RrGO5qszNl0g?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>MTsN 3 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MTsN+3+Banyuwangi/data=!4m7!3m6!1s0x2dd3fded279bd40f:0x658f85ccdcf96342!8m2!3d-8.4031164!4d114.2621832!16s%2Fg%2F1hm5gqt5w!19sChIJD9SbJ-390y0RQmP53MyFj2U?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>SMP Negeri 4 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Negeri+4+Banyuwangi/data=!4m7!3m6!1s0x2dd1453be2d1f7b9:0x19beb00ed2c3048e!8m2!3d-8.2070793!4d114.364183!16s%2Fg%2F11b7dx0ktr!19sChIJuffR4jtF0S0RjgTD0g6wvhk?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Sekolah</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah/data=!4m7!3m6!1s0x2dd3ff77edf2c4e9:0x2c3ac2699a227f94!8m2!3d-8.4702768!4d114.2235516!16s%2Fg%2F11shp_6bls!19sChIJ6cTy7Xf_0y0RlH8immnCOiw?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Amanah Edu Centre</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Amanah+Edu+Centre/data=!4m7!3m6!1s0x2dd15ac599d9c1e5:0x360c3cc817fe9871!8m2!3d-8.2327563!4d114.3661416!16s%2Fg%2F11dyrc9zc2!19sChIJ5cHZmcVa0S0RcZj-F8g8DDY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>KUMON BANYUWANGI</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/KUMON+BANYUWANGI/data=!4m7!3m6!1s0x2dd145322a9956bd:0x8a1f59d443a7818f!8m2!3d-8.2162198!4d114.3668366!16s%2Fg%2F11fzsdxp7v!19sChIJvVaZKjJF0S0Rj4GnQ9RZH4o?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>KB AL IRSYAD AL ISLAMIYYAH Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/KB+AL+IRSYAD+AL+ISLAMIYYAH+Banyuwangi/data=!4m7!3m6!1s0x2dd145221df6b7dd:0xc6d658e3f6954a00!8m2!3d-8.2017676!4d114.3755326!16s%2Fg%2F1pzsq20y6!19sChIJ3bf2HSJF0S0RAEqV9uNY1sY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Bina Insan Qurani - Belajar Al Quran dan Ilmu Qiraat di Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bina+Insan+Qurani+-+Belajar+Al+Quran+dan+Ilmu+Qiraat+di+Banyuwangi/data=!4m7!3m6!1s0x2dd15b7cd2699847:0xd1be716a65f7a8cc!8m2!3d-8.2277844!4d114.3656062!16s%2Fg%2F11t3g9hq8j!19sChIJR5hp0nxb0S0RzKj3ZWpxvtE?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>SDLB A Negeri Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SDLB+A+Negeri+Banyuwangi/data=!4m7!3m6!1s0x2dd14545927d4fa5:0x217ba42f47351ed4!8m2!3d-8.2117872!4d114.3502521!16s%2Fg%2F11b6hv6kf8!19sChIJpU99kkVF0S0R1B41Ry-keyE?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Dinas Pendidikan Kabupaten Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Dinas+Pendidikan+Kabupaten+Banyuwangi/data=!4m7!3m6!1s0x2dd15ac90617a827:0x70991cbaed68fc65!8m2!3d-8.2285884!4d114.3613779!16s%2Fg%2F1hc1jdm99!19sChIJJ6gXBsla0S0RZfxo7bocmXA?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>SMP Muhammadiyah 3 Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Muhammadiyah+3+Banyuwangi/data=!4m7!3m6!1s0x2dd14536abbb5803:0x51989194972727ec!8m2!3d-8.216271!4d114.3635744!16s%2Fg%2F11bc7n_995!19sChIJA1i7qzZF0S0R7Ccnl5SRmFE?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Sekolah Menengah Atas PGRI Rogojampi</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+Menengah+Atas+PGRI+Rogojampi/data=!4m7!3m6!1s0x2dd145259a829f79:0xd2e648308ddf67fb!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F11b6d40qf5!19sChIJeZ-CmiVF0S0R-2ffjTBI5tI?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>LKP PTCC BANYUWANGI</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/LKP+PTCC+BANYUWANGI/data=!4m7!3m6!1s0x2dd145485a21eec1:0x22130602de80d324!8m2!3d-8.2140143!4d114.3553138!16s%2Fg%2F11bv3v_tqx!19sChIJwe4hWkhF0S0RJNOA3gIGEyI?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>SDN 1 Karangrejo Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SDN+1+Karangrejo+Banyuwangi/data=!4m7!3m6!1s0x2dd145dc2c5f146b:0xf8558a3b763a84f3!8m2!3d-8.2189716!4d114.3783573!16s%2Fg%2F11grb6hrng!19sChIJaxRfLNxF0S0R84Q6djuKVfg?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>SMP PGRI Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+PGRI+Banyuwangi/data=!4m7!3m6!1s0x2dd14532ccb604e3:0x7696c125f5aa4d0f!8m2!3d-8.2213677!4d114.3680288!16s%2Fg%2F1hm4rcqvb!19sChIJ4wS2zDJF0S0RD02q9SXBlnY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Universitas Bakti Indonesia UBI</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Universitas+Bakti+Indonesia+UBI/data=!4m7!3m6!1s0x2dd3fddcd48b307b:0xefae92787267e033!8m2!3d-8.4132676!4d114.2503667!16s%2Fg%2F1hm5xg7r5!19sChIJezCL1Nz90y0RM-BncniSru8?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>RA Baiturrahman 1</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/RA+Baiturrahman+1/data=!4m7!3m6!1s0x2dd145259fe7692d:0x3e41724d573b33ae!8m2!3d-8.2098497!4d114.3727227!16s%2Fg%2F11f54yq18f!19sChIJLWnnnyVF0S0RrjM7V01yQT4?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Madrasah Aliyah Darul Huda Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Madrasah+Aliyah+Darul+Huda+Banyuwangi/data=!4m7!3m6!1s0x2dd145259a829f79:0x8ea54f2bee2a6dd4!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F1pzx7z__h!19sChIJeZ-CmiVF0S0R1G0q7itPpY4?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>TK PAUD RA Qur'an Tunas Ceria Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TK+PAUD+RA+Qur%27an+Tunas+Ceria+Banyuwangi/data=!4m7!3m6!1s0x2dd15bba5f766d23:0xb0a703849f613b75!8m2!3d-8.2230927!4d114.3749979!16s%2Fg%2F11s_v8nkbm!19sChIJI212X7pb0S0RdTthn4QDp7A?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>SMP Negeri 2 Kalipuro Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Negeri+2+Kalipuro+Banyuwangi/data=!4m7!3m6!1s0x2dd1459f05a36f89:0xa3284e9d694a48bc!8m2!3d-8.1792488!4d114.3556002!16s%2Fg%2F11cjqsrbm1!19sChIJiW-jBZ9F0S0RvEhKaZ1OKKM?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>MA Muhammadiyah 1 Pakis Duren Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MA+Muhammadiyah+1+Pakis+Duren+Banyuwangi/data=!4m7!3m6!1s0x2dd15a94a2f06565:0x1653ef1e3f93799b!8m2!3d-8.2466703!4d114.3569188!16s%2Fg%2F11bv1tfnm6!19sChIJZWXwopRa0S0Rm3mTPx7vUxY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>ISLAMIC CENTER BAITURRAHMAN BANYUWANGI</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/ISLAMIC+CENTER+BAITURRAHMAN+BANYUWANGI/data=!4m7!3m6!1s0x2dd14532b712a7eb:0xffcb1c8b8c0dd1c3!8m2!3d-8.2215398!4d114.3684359!16s%2Fg%2F11fyzfck5m!19sChIJ66cStzJF0S0Rw9ENjIscy_8?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>SMP Al Irsyad Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SMP+Al+Irsyad+Banyuwangi/data=!4m7!3m6!1s0x2dd1452f4d410c83:0x1139a1b0b4a03c0e!8m2!3d-8.20175!4d114.373382!16s%2Fg%2F1hm50j_ll!19sChIJgwxBTS9F0S0RDjygtLChORE?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>PAUD Inklusif Cerdas Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/PAUD+Inklusif+Cerdas+Banyuwangi/data=!4m7!3m6!1s0x2dd15ad21d808dc9:0xab22893fecba993c!8m2!3d-8.2263348!4d114.3706854!16s%2Fg%2F1hm4_052f!19sChIJyY2AHdJa0S0RPJm67D-JIqs?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>TK Santa Maria Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TK+Santa+Maria+Banyuwangi/data=!4m7!3m6!1s0x2dd145007f3b04bf:0x174eacfc95d2b82f!8m2!3d-8.2164652!4d114.3605725!16s%2Fg%2F11vt1vzyr2!19sChIJvwQ7fwBF0S0RL7jSlfysThc?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>SD Negeri 1 Mojopanggung</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SD+Negeri+1+Mojopanggung/data=!4m7!3m6!1s0x2dd1454f4b278033:0x46c4d0c9f064d7e8!8m2!3d-8.2136487!4d114.3520271!16s%2Fg%2F1hm2wwfb3!19sChIJM4AnS09F0S0R6Ndk8MnQxEY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Slb pgri banyuwangi</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Slb+pgri+banyuwangi/data=!4m7!3m6!1s0x2dd15b9d35320fab:0xc51fd8319f95490c!8m2!3d-8.2328665!4d114.3573342!16s%2Fg%2F11sw6y6blp!19sChIJqw8yNZ1b0S0RDEmVnzHYH8U?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>TK Islam Rahmatullah</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TK+Islam+Rahmatullah/data=!4m7!3m6!1s0x2dd15abf704d0189:0x36629cc02e1ffecd!8m2!3d-8.2258982!4d114.3615134!16s%2Fg%2F1pzw8hgz1!19sChIJiQFNcL9a0S0Rzf4fLsCcYjY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>PT. Banyuwangi Jaya Sejahtera Abadi</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/PT.+Banyuwangi+Jaya+Sejahtera+Abadi/data=!4m7!3m6!1s0x2dd15bb261818cab:0x22f19bcc010c9700!8m2!3d-8.2325184!4d114.3668383!16s%2Fg%2F11h0vt12dk!19sChIJq4yBYbJb0S0RAJcMAcyb8SI?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>SD Negeri 1 Penganjuran</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SD+Negeri+1+Penganjuran/data=!4m7!3m6!1s0x2dd14533da0a0667:0x7f0da9d1aed1bf75!8m2!3d-8.2170631!4d114.3657983!16s%2Fg%2F11c0t9g08f!19sChIJZwYK2jNF0S0Rdb_RrtGpDX8?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Sekolah Menengah Kejuruan Muhammadiyah 1 Genteng</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Sekolah+Menengah+Kejuruan+Muhammadiyah+1+Genteng/data=!4m7!3m6!1s0x2dd145259a829f79:0x37575410654e69c3!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F1pzvl3w1w!19sChIJeZ-CmiVF0S0Rw2lOZRBUVzc?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Kadek Modelling School</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Kadek+Modelling+School/data=!4m7!3m6!1s0x2dd1452e5dd3ab6f:0xb24335f9b53b1570!8m2!3d-8.2143758!4d114.3723035!16s%2Fg%2F11bc7szxtq!19sChIJb6vTXS5F0S0RcBU7tfk1Q7I?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Madrasah Ibtidaiyah Islamiyah Sumber Beras Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Madrasah+Ibtidaiyah+Islamiyah+Sumber+Beras+Banyuwangi/data=!4m7!3m6!1s0x2dd145259a829f79:0xbeb4ee66c7af3e45!8m2!3d-8.2102562!4d114.3735107!16s%2Fg%2F1pzrz6k4n!19sChIJeZ-CmiVF0S0RRT6vx2butL4?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>SDN 1 Rejosari Glagah Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/SDN+1+Rejosari+Glagah+Banyuwangi/data=!4m7!3m6!1s0x2dd1500085e26a19:0xa3e3c86706591df4!8m2!3d-8.2264946!4d114.3334813!16s%2Fg%2F11cm_4v0zh!19sChIJGWrihQBQ0S0R9B1ZBmfI46M?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>TK AISYIYAH BUSTANUL ATHFAL I</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/TK+AISYIYAH+BUSTANUL+ATHFAL+I/data=!4m7!3m6!1s0x2dd15ac8d3dc0d55:0xc63191fa314957fd!8m2!3d-8.2278984!4d114.3644779!16s%2Fg%2F1pzrxnvhl!19sChIJVQ3c08ha0S0R_VdJMfqRMcY?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Askar Kauny Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Askar+Kauny+Banyuwangi/data=!4m7!3m6!1s0x2dd15ac4367a13f5:0xca82bad30a719304!8m2!3d-8.2349813!4d114.3658961!16s%2Fg%2F11df80g1hc!19sChIJ9RN6NsRa0S0RBJNxCtO6gso?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>MM Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/MM+Banyuwangi/data=!4m7!3m6!1s0x2dd15b42c7e875b1:0x8b9fdf89caeadca8!8m2!3d-8.2264533!4d114.3587519!16s%2Fg%2F11rw6dljv5!19sChIJsXXox0Jb0S0RqNzqyonfn4s?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Bintang junior bimba kids banyuwangi</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Bintang+junior+bimba+kids+banyuwangi/data=!4m7!3m6!1s0x2dd15b092fc647e3:0xe0711ea0d15a787b!8m2!3d-8.2252457!4d114.371453!16s%2Fg%2F11rtqdqpj0!19sChIJ40fGLwlb0S0Re3ha0aAeceA?authuser=0&amp;hl=id&amp;rclk=1</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Masjid Besar KH. Ahmad Dahlan Banyuwangi</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Tidak ditemukan</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>https://www.google.com/maps/place/Masjid+Besar+KH.+Ahmad+Dahlan+Banyuwangi/data=!4m7!3m6!1s0x2dd15ac8542771d5:0x83177d78bc0677b3!8m2!3d-8.2280298!4d114.3647626!16s%2Fg%2F1pzsld363!19sChIJ1XEnVMha0S0Rs3cGvHh9F4M?authuser=0&amp;hl=id&amp;rclk=1</t>
         </is>
       </c>
     </row>

</xml_diff>